<commit_message>
unit selection & move commands
</commit_message>
<xml_diff>
--- a/src/Wizard Tower.xlsx
+++ b/src/Wizard Tower.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian Payton\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian Payton\Documents\GameMakerStudio2\WizardTower\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F8C2FE-04E2-4F68-800D-80C5EB142625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A879865-563B-43B6-BE52-F067AF61CF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3B572C5C-39EA-4FDC-AE92-C6809A967981}"/>
+    <workbookView xWindow="29370" yWindow="3315" windowWidth="21600" windowHeight="11505" xr2:uid="{3B572C5C-39EA-4FDC-AE92-C6809A967981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890B95B1-4562-4257-9EDB-A907204B7FCE}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
putting in all the units and structures that were planned
</commit_message>
<xml_diff>
--- a/src/Wizard Tower.xlsx
+++ b/src/Wizard Tower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian Payton\Documents\GameMakerStudio2\WizardTower\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A879865-563B-43B6-BE52-F067AF61CF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9304CF-9F87-49BC-B46C-B926EE8B6918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="3315" windowWidth="21600" windowHeight="11505" xr2:uid="{3B572C5C-39EA-4FDC-AE92-C6809A967981}"/>
+    <workbookView xWindow="3885" yWindow="480" windowWidth="21600" windowHeight="12750" xr2:uid="{3B572C5C-39EA-4FDC-AE92-C6809A967981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>WIZARD TOWER</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Less Idling than other Tower Defense</t>
+  </si>
+  <si>
+    <t>tower</t>
+  </si>
+  <si>
+    <t>basic attack structure, fires magic missiles to damage enemies.  Can be upgraded into three different tower types (flame, bolt, or ice)</t>
   </si>
 </sst>
 </file>
@@ -248,8 +254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{108ECF09-9CFD-45B6-AC95-6C3D1451381E}" name="Table1" displayName="Table1" ref="A2:K8" totalsRowShown="0">
-  <autoFilter ref="A2:K8" xr:uid="{108ECF09-9CFD-45B6-AC95-6C3D1451381E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{108ECF09-9CFD-45B6-AC95-6C3D1451381E}" name="Table1" displayName="Table1" ref="A2:K9" totalsRowShown="0">
+  <autoFilter ref="A2:K9" xr:uid="{108ECF09-9CFD-45B6-AC95-6C3D1451381E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{41E4E6C8-44E3-4B32-9C50-F6660EBD2E12}" name="Buildings" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{FD491E72-DFAF-4A4A-A651-7C7EC5592EDA}" name="Description" dataDxfId="0"/>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890B95B1-4562-4257-9EDB-A907204B7FCE}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,79 +692,89 @@
     </row>
     <row r="6" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="2"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>